<commit_message>
fix E3ME reporting, add mod mean plot
</commit_message>
<xml_diff>
--- a/model_results/E3ME-FTT data for NAVIGATE Task 4.2_V5.xlsx
+++ b/model_results/E3ME-FTT data for NAVIGATE Task 4.2_V5.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE435DD2-B6C1-48CE-BBD6-3FB01AA791E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77139DC8-214F-4748-B054-9E0AF48934DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="740" windowWidth="19180" windowHeight="11260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="-108" windowWidth="30936" windowHeight="17496" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$1726</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$O$1076</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -670,8 +670,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1726"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" topLeftCell="A619" workbookViewId="0">
+      <selection activeCell="H805" sqref="H805"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -42550,7 +42550,7 @@
         <v>5</v>
       </c>
       <c r="B952" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C952" s="13" t="s">
         <v>14</v>
@@ -42594,7 +42594,7 @@
         <v>5</v>
       </c>
       <c r="B953" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C953" s="13" t="s">
         <v>14</v>
@@ -42638,7 +42638,7 @@
         <v>5</v>
       </c>
       <c r="B954" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C954" s="13" t="s">
         <v>14</v>
@@ -42682,7 +42682,7 @@
         <v>5</v>
       </c>
       <c r="B955" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C955" s="13" t="s">
         <v>14</v>
@@ -42726,7 +42726,7 @@
         <v>5</v>
       </c>
       <c r="B956" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C956" s="13" t="s">
         <v>14</v>

</xml_diff>